<commit_message>
The data is now consumed. Something is wrong with the self.executor.submit part in _consumer_loop
</commit_message>
<xml_diff>
--- a/data_preparation/data/final_signals_info.xlsx
+++ b/data_preparation/data/final_signals_info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="262">
   <si>
     <t>caseid</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>e2f106bcdad78e1c8f19c663d4d4f168c90e8c1b</t>
-  </si>
-  <si>
-    <t>0ed1f6a51b46c3f6436e61b2abc69079eb9bcf2c</t>
   </si>
   <si>
     <t>f27bd1a9530001517ac25aab6a3bdd726ec56942</t>
@@ -810,7 +807,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,13 +817,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -881,7 +872,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1195,7 +1186,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D237"/>
+  <dimension ref="A1:D236"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1221,7 +1212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>609</v>
       </c>
@@ -1235,7 +1226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>609</v>
       </c>
@@ -1249,7 +1240,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3">
         <v>609</v>
       </c>
@@ -1263,7 +1254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3">
         <v>609</v>
       </c>
@@ -1277,7 +1268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3">
         <v>609</v>
       </c>
@@ -1291,7 +1282,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3">
         <v>609</v>
       </c>
@@ -1305,7 +1296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3">
         <v>634</v>
       </c>
@@ -1319,7 +1310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3">
         <v>634</v>
       </c>
@@ -1333,7 +1324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>634</v>
       </c>
@@ -1347,7 +1338,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3">
         <v>634</v>
       </c>
@@ -1361,7 +1352,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3">
         <v>634</v>
       </c>
@@ -1375,7 +1366,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3">
         <v>634</v>
       </c>
@@ -1557,7 +1548,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3">
         <v>1032</v>
       </c>
@@ -1571,7 +1562,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3">
         <v>1087</v>
       </c>
@@ -1585,7 +1576,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3">
         <v>1087</v>
       </c>
@@ -1599,7 +1590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3">
         <v>1087</v>
       </c>
@@ -1613,7 +1604,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3">
         <v>1087</v>
       </c>
@@ -1627,7 +1618,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3">
         <v>1087</v>
       </c>
@@ -1641,7 +1632,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3">
         <v>1087</v>
       </c>
@@ -1655,7 +1646,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3">
         <v>1087</v>
       </c>
@@ -1669,253 +1660,253 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="3">
         <v>1087</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3">
         <v>1087</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="3">
-        <v>1087</v>
+        <v>1209</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="3">
         <v>1209</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="3">
         <v>1209</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="3">
         <v>1209</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="3">
         <v>1209</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="3">
         <v>1209</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="3">
         <v>1209</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="3">
         <v>1209</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="3">
         <v>1209</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="3">
-        <v>1209</v>
+        <v>1488</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="3">
         <v>1488</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="3">
         <v>1488</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="3">
         <v>1488</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="3">
         <v>1488</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="3">
         <v>1488</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="3">
         <v>1488</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>73</v>
@@ -1926,10 +1917,10 @@
         <v>1488</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>74</v>
@@ -1940,10 +1931,10 @@
         <v>1488</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>75</v>
@@ -1954,10 +1945,10 @@
         <v>1488</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>76</v>
@@ -1965,13 +1956,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3">
-        <v>1488</v>
+        <v>1903</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>77</v>
@@ -1982,10 +1973,10 @@
         <v>1903</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>78</v>
@@ -1996,10 +1987,10 @@
         <v>1903</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>79</v>
@@ -2010,10 +2001,10 @@
         <v>1903</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>80</v>
@@ -2024,10 +2015,10 @@
         <v>1903</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>81</v>
@@ -2038,10 +2029,10 @@
         <v>1903</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>82</v>
@@ -2052,10 +2043,10 @@
         <v>1903</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>83</v>
@@ -2066,10 +2057,10 @@
         <v>1903</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>84</v>
@@ -2080,10 +2071,10 @@
         <v>1903</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>85</v>
@@ -2094,10 +2085,10 @@
         <v>1903</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>86</v>
@@ -2105,13 +2096,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3">
-        <v>1903</v>
+        <v>1952</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>87</v>
@@ -2122,10 +2113,10 @@
         <v>1952</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>88</v>
@@ -2136,10 +2127,10 @@
         <v>1952</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>89</v>
@@ -2150,10 +2141,10 @@
         <v>1952</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>90</v>
@@ -2164,10 +2155,10 @@
         <v>1952</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>91</v>
@@ -2178,10 +2169,10 @@
         <v>1952</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>92</v>
@@ -2189,13 +2180,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3">
-        <v>1952</v>
+        <v>2191</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>93</v>
@@ -2206,10 +2197,10 @@
         <v>2191</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>94</v>
@@ -2220,10 +2211,10 @@
         <v>2191</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>95</v>
@@ -2234,10 +2225,10 @@
         <v>2191</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>96</v>
@@ -2248,10 +2239,10 @@
         <v>2191</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>97</v>
@@ -2262,10 +2253,10 @@
         <v>2191</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>98</v>
@@ -2273,13 +2264,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3">
-        <v>2191</v>
+        <v>2259</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>99</v>
@@ -2290,10 +2281,10 @@
         <v>2259</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>100</v>
@@ -2304,10 +2295,10 @@
         <v>2259</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>101</v>
@@ -2318,10 +2309,10 @@
         <v>2259</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>102</v>
@@ -2332,10 +2323,10 @@
         <v>2259</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>103</v>
@@ -2346,10 +2337,10 @@
         <v>2259</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>104</v>
@@ -2357,13 +2348,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3">
-        <v>2259</v>
+        <v>2327</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>105</v>
@@ -2374,10 +2365,10 @@
         <v>2327</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>106</v>
@@ -2388,10 +2379,10 @@
         <v>2327</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>107</v>
@@ -2402,13 +2393,13 @@
         <v>2327</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
@@ -2416,10 +2407,10 @@
         <v>2327</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>110</v>
@@ -2430,10 +2421,10 @@
         <v>2327</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>111</v>
@@ -2444,10 +2435,10 @@
         <v>2327</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>112</v>
@@ -2458,10 +2449,10 @@
         <v>2327</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>113</v>
@@ -2472,10 +2463,10 @@
         <v>2327</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>114</v>
@@ -2486,24 +2477,24 @@
         <v>2327</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3">
-        <v>2327</v>
+        <v>2340</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>117</v>
@@ -2514,10 +2505,10 @@
         <v>2340</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>118</v>
@@ -2528,10 +2519,10 @@
         <v>2340</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>119</v>
@@ -2542,10 +2533,10 @@
         <v>2340</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>120</v>
@@ -2556,10 +2547,10 @@
         <v>2340</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>121</v>
@@ -2570,10 +2561,10 @@
         <v>2340</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>122</v>
@@ -2584,10 +2575,10 @@
         <v>2340</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>123</v>
@@ -2598,10 +2589,10 @@
         <v>2340</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>124</v>
@@ -2612,10 +2603,10 @@
         <v>2340</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>125</v>
@@ -2626,10 +2617,10 @@
         <v>2340</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>126</v>
@@ -2637,13 +2628,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="3">
-        <v>2340</v>
+        <v>2422</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>127</v>
@@ -2654,10 +2645,10 @@
         <v>2422</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>128</v>
@@ -2668,10 +2659,10 @@
         <v>2422</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>129</v>
@@ -2682,10 +2673,10 @@
         <v>2422</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>130</v>
@@ -2696,10 +2687,10 @@
         <v>2422</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>131</v>
@@ -2710,10 +2701,10 @@
         <v>2422</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>132</v>
@@ -2724,10 +2715,10 @@
         <v>2422</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>133</v>
@@ -2738,10 +2729,10 @@
         <v>2422</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>134</v>
@@ -2752,10 +2743,10 @@
         <v>2422</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>135</v>
@@ -2763,13 +2754,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="3">
-        <v>2422</v>
+        <v>2626</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>136</v>
@@ -2780,10 +2771,10 @@
         <v>2626</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>137</v>
@@ -2794,10 +2785,10 @@
         <v>2626</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>138</v>
@@ -2808,10 +2799,10 @@
         <v>2626</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>139</v>
@@ -2822,10 +2813,10 @@
         <v>2626</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>140</v>
@@ -2836,10 +2827,10 @@
         <v>2626</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>141</v>
@@ -2847,13 +2838,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="3">
-        <v>2626</v>
+        <v>2724</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>142</v>
@@ -2864,10 +2855,10 @@
         <v>2724</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>143</v>
@@ -2878,10 +2869,10 @@
         <v>2724</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>144</v>
@@ -2892,10 +2883,10 @@
         <v>2724</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>145</v>
@@ -2906,10 +2897,10 @@
         <v>2724</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>146</v>
@@ -2920,10 +2911,10 @@
         <v>2724</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>147</v>
@@ -2934,10 +2925,10 @@
         <v>2724</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>148</v>
@@ -2948,10 +2939,10 @@
         <v>2724</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>149</v>
@@ -2962,10 +2953,10 @@
         <v>2724</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>150</v>
@@ -2973,13 +2964,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="3">
-        <v>2724</v>
+        <v>2880</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>151</v>
@@ -2990,10 +2981,10 @@
         <v>2880</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>152</v>
@@ -3004,10 +2995,10 @@
         <v>2880</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>153</v>
@@ -3018,10 +3009,10 @@
         <v>2880</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>154</v>
@@ -3032,10 +3023,10 @@
         <v>2880</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>155</v>
@@ -3046,10 +3037,10 @@
         <v>2880</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>156</v>
@@ -3057,13 +3048,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="3">
-        <v>2880</v>
+        <v>3519</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D133" s="4" t="s">
         <v>157</v>
@@ -3074,10 +3065,10 @@
         <v>3519</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D134" s="4" t="s">
         <v>158</v>
@@ -3088,10 +3079,10 @@
         <v>3519</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>159</v>
@@ -3102,10 +3093,10 @@
         <v>3519</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D136" s="4" t="s">
         <v>160</v>
@@ -3116,10 +3107,10 @@
         <v>3519</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D137" s="4" t="s">
         <v>161</v>
@@ -3130,10 +3121,10 @@
         <v>3519</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D138" s="4" t="s">
         <v>162</v>
@@ -3144,10 +3135,10 @@
         <v>3519</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D139" s="4" t="s">
         <v>163</v>
@@ -3158,10 +3149,10 @@
         <v>3519</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D140" s="4" t="s">
         <v>164</v>
@@ -3172,10 +3163,10 @@
         <v>3519</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D141" s="4" t="s">
         <v>165</v>
@@ -3186,10 +3177,10 @@
         <v>3519</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D142" s="4" t="s">
         <v>166</v>
@@ -3197,13 +3188,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="3">
-        <v>3519</v>
+        <v>3638</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D143" s="4" t="s">
         <v>167</v>
@@ -3214,10 +3205,10 @@
         <v>3638</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>168</v>
@@ -3228,10 +3219,10 @@
         <v>3638</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>169</v>
@@ -3242,10 +3233,10 @@
         <v>3638</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>170</v>
@@ -3256,10 +3247,10 @@
         <v>3638</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D147" s="4" t="s">
         <v>171</v>
@@ -3270,10 +3261,10 @@
         <v>3638</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D148" s="4" t="s">
         <v>172</v>
@@ -3281,13 +3272,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
       <c r="A149" s="3">
-        <v>3638</v>
+        <v>3984</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D149" s="4" t="s">
         <v>173</v>
@@ -3298,10 +3289,10 @@
         <v>3984</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D150" s="4" t="s">
         <v>174</v>
@@ -3312,10 +3303,10 @@
         <v>3984</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D151" s="4" t="s">
         <v>175</v>
@@ -3326,10 +3317,10 @@
         <v>3984</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D152" s="4" t="s">
         <v>176</v>
@@ -3340,10 +3331,10 @@
         <v>3984</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>177</v>
@@ -3354,10 +3345,10 @@
         <v>3984</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>178</v>
@@ -3365,16 +3356,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
       <c r="A155" s="3">
-        <v>3984</v>
+        <v>4658</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
@@ -3382,10 +3373,10 @@
         <v>4658</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>181</v>
@@ -3396,10 +3387,10 @@
         <v>4658</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>182</v>
@@ -3410,10 +3401,10 @@
         <v>4658</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D158" s="4" t="s">
         <v>183</v>
@@ -3424,10 +3415,10 @@
         <v>4658</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="D159" s="4" t="s">
         <v>184</v>
@@ -3438,10 +3429,10 @@
         <v>4658</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>185</v>
@@ -3452,10 +3443,10 @@
         <v>4658</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D161" s="4" t="s">
         <v>186</v>
@@ -3466,10 +3457,10 @@
         <v>4658</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D162" s="4" t="s">
         <v>187</v>
@@ -3480,10 +3471,10 @@
         <v>4658</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D163" s="4" t="s">
         <v>188</v>
@@ -3491,13 +3482,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
       <c r="A164" s="3">
-        <v>4658</v>
+        <v>4721</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D164" s="4" t="s">
         <v>189</v>
@@ -3508,10 +3499,10 @@
         <v>4721</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D165" s="4" t="s">
         <v>190</v>
@@ -3522,10 +3513,10 @@
         <v>4721</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D166" s="4" t="s">
         <v>191</v>
@@ -3536,10 +3527,10 @@
         <v>4721</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D167" s="4" t="s">
         <v>192</v>
@@ -3550,10 +3541,10 @@
         <v>4721</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D168" s="4" t="s">
         <v>193</v>
@@ -3564,10 +3555,10 @@
         <v>4721</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D169" s="4" t="s">
         <v>194</v>
@@ -3578,10 +3569,10 @@
         <v>4721</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D170" s="4" t="s">
         <v>195</v>
@@ -3592,10 +3583,10 @@
         <v>4721</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D171" s="4" t="s">
         <v>196</v>
@@ -3606,10 +3597,10 @@
         <v>4721</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D172" s="4" t="s">
         <v>197</v>
@@ -3620,10 +3611,10 @@
         <v>4721</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D173" s="4" t="s">
         <v>198</v>
@@ -3631,13 +3622,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="3">
-        <v>4721</v>
+        <v>4978</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D174" s="4" t="s">
         <v>199</v>
@@ -3648,10 +3639,10 @@
         <v>4978</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D175" s="4" t="s">
         <v>200</v>
@@ -3662,10 +3653,10 @@
         <v>4978</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D176" s="4" t="s">
         <v>201</v>
@@ -3676,10 +3667,10 @@
         <v>4978</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D177" s="4" t="s">
         <v>202</v>
@@ -3690,10 +3681,10 @@
         <v>4978</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D178" s="4" t="s">
         <v>203</v>
@@ -3704,10 +3695,10 @@
         <v>4978</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D179" s="4" t="s">
         <v>204</v>
@@ -3715,13 +3706,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="3">
-        <v>4978</v>
+        <v>5107</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D180" s="4" t="s">
         <v>205</v>
@@ -3732,10 +3723,10 @@
         <v>5107</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D181" s="4" t="s">
         <v>206</v>
@@ -3746,10 +3737,10 @@
         <v>5107</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D182" s="4" t="s">
         <v>207</v>
@@ -3760,10 +3751,10 @@
         <v>5107</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D183" s="4" t="s">
         <v>208</v>
@@ -3774,10 +3765,10 @@
         <v>5107</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D184" s="4" t="s">
         <v>209</v>
@@ -3788,10 +3779,10 @@
         <v>5107</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D185" s="4" t="s">
         <v>210</v>
@@ -3802,10 +3793,10 @@
         <v>5107</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D186" s="4" t="s">
         <v>211</v>
@@ -3816,10 +3807,10 @@
         <v>5107</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D187" s="4" t="s">
         <v>212</v>
@@ -3830,10 +3821,10 @@
         <v>5107</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D188" s="4" t="s">
         <v>213</v>
@@ -3844,10 +3835,10 @@
         <v>5107</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D189" s="4" t="s">
         <v>214</v>
@@ -3855,13 +3846,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="3">
-        <v>5107</v>
+        <v>5211</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D190" s="4" t="s">
         <v>215</v>
@@ -3872,10 +3863,10 @@
         <v>5211</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D191" s="4" t="s">
         <v>216</v>
@@ -3886,10 +3877,10 @@
         <v>5211</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D192" s="4" t="s">
         <v>217</v>
@@ -3900,10 +3891,10 @@
         <v>5211</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D193" s="4" t="s">
         <v>218</v>
@@ -3914,10 +3905,10 @@
         <v>5211</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D194" s="4" t="s">
         <v>219</v>
@@ -3928,10 +3919,10 @@
         <v>5211</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D195" s="4" t="s">
         <v>220</v>
@@ -3939,13 +3930,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
       <c r="A196" s="3">
-        <v>5211</v>
+        <v>5248</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D196" s="4" t="s">
         <v>221</v>
@@ -3956,10 +3947,10 @@
         <v>5248</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D197" s="4" t="s">
         <v>222</v>
@@ -3970,10 +3961,10 @@
         <v>5248</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D198" s="4" t="s">
         <v>223</v>
@@ -3984,10 +3975,10 @@
         <v>5248</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D199" s="4" t="s">
         <v>224</v>
@@ -3998,10 +3989,10 @@
         <v>5248</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D200" s="4" t="s">
         <v>225</v>
@@ -4012,10 +4003,10 @@
         <v>5248</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D201" s="4" t="s">
         <v>226</v>
@@ -4023,13 +4014,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
       <c r="A202" s="3">
-        <v>5248</v>
+        <v>5337</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D202" s="4" t="s">
         <v>227</v>
@@ -4040,10 +4031,10 @@
         <v>5337</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D203" s="4" t="s">
         <v>228</v>
@@ -4054,10 +4045,10 @@
         <v>5337</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D204" s="4" t="s">
         <v>229</v>
@@ -4068,10 +4059,10 @@
         <v>5337</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D205" s="4" t="s">
         <v>230</v>
@@ -4082,10 +4073,10 @@
         <v>5337</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D206" s="4" t="s">
         <v>231</v>
@@ -4096,10 +4087,10 @@
         <v>5337</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D207" s="4" t="s">
         <v>232</v>
@@ -4107,13 +4098,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
       <c r="A208" s="3">
-        <v>5337</v>
+        <v>5540</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D208" s="4" t="s">
         <v>233</v>
@@ -4124,10 +4115,10 @@
         <v>5540</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D209" s="4" t="s">
         <v>234</v>
@@ -4138,10 +4129,10 @@
         <v>5540</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D210" s="4" t="s">
         <v>235</v>
@@ -4152,10 +4143,10 @@
         <v>5540</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D211" s="4" t="s">
         <v>236</v>
@@ -4166,10 +4157,10 @@
         <v>5540</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D212" s="4" t="s">
         <v>237</v>
@@ -4180,10 +4171,10 @@
         <v>5540</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D213" s="4" t="s">
         <v>238</v>
@@ -4191,13 +4182,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="18.75">
       <c r="A214" s="3">
-        <v>5540</v>
+        <v>5841</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D214" s="4" t="s">
         <v>239</v>
@@ -4208,10 +4199,10 @@
         <v>5841</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D215" s="4" t="s">
         <v>240</v>
@@ -4222,10 +4213,10 @@
         <v>5841</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D216" s="4" t="s">
         <v>241</v>
@@ -4233,13 +4224,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
       <c r="A217" s="3">
-        <v>5841</v>
+        <v>6234</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D217" s="4" t="s">
         <v>242</v>
@@ -4250,10 +4241,10 @@
         <v>6234</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D218" s="4" t="s">
         <v>243</v>
@@ -4264,10 +4255,10 @@
         <v>6234</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D219" s="4" t="s">
         <v>244</v>
@@ -4278,10 +4269,10 @@
         <v>6234</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D220" s="4" t="s">
         <v>245</v>
@@ -4292,10 +4283,10 @@
         <v>6234</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D221" s="4" t="s">
         <v>246</v>
@@ -4306,10 +4297,10 @@
         <v>6234</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D222" s="4" t="s">
         <v>247</v>
@@ -4320,10 +4311,10 @@
         <v>6234</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D223" s="4" t="s">
         <v>248</v>
@@ -4334,10 +4325,10 @@
         <v>6234</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D224" s="4" t="s">
         <v>249</v>
@@ -4348,10 +4339,10 @@
         <v>6234</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D225" s="4" t="s">
         <v>250</v>
@@ -4362,10 +4353,10 @@
         <v>6234</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D226" s="4" t="s">
         <v>251</v>
@@ -4373,13 +4364,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="18.75">
       <c r="A227" s="3">
-        <v>6234</v>
+        <v>6335</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D227" s="4" t="s">
         <v>252</v>
@@ -4390,10 +4381,10 @@
         <v>6335</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D228" s="4" t="s">
         <v>253</v>
@@ -4404,10 +4395,10 @@
         <v>6335</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D229" s="4" t="s">
         <v>254</v>
@@ -4418,10 +4409,10 @@
         <v>6335</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D230" s="4" t="s">
         <v>255</v>
@@ -4432,10 +4423,10 @@
         <v>6335</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D231" s="4" t="s">
         <v>256</v>
@@ -4446,10 +4437,10 @@
         <v>6335</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D232" s="4" t="s">
         <v>257</v>
@@ -4460,10 +4451,10 @@
         <v>6335</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D233" s="4" t="s">
         <v>258</v>
@@ -4474,10 +4465,10 @@
         <v>6335</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D234" s="4" t="s">
         <v>259</v>
@@ -4488,10 +4479,10 @@
         <v>6335</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D235" s="4" t="s">
         <v>260</v>
@@ -4502,27 +4493,13 @@
         <v>6335</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D236" s="4" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="18.75">
-      <c r="A237" s="3">
-        <v>6335</v>
-      </c>
-      <c r="B237" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C237" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D237" s="4" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>